<commit_message>
TCVM  case study  commit
</commit_message>
<xml_diff>
--- a/src/main/resources/excelFiles/report.xlsx
+++ b/src/main/resources/excelFiles/report.xlsx
@@ -79,10 +79,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>104.0</v>
+        <v>111.0</v>
       </c>
       <c r="C1" t="n">
-        <v>1040.0</v>
+        <v>1110.0</v>
       </c>
     </row>
     <row r="2">
@@ -101,10 +101,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>26.0</v>
+        <v>31.0</v>
       </c>
       <c r="C3" t="n">
-        <v>390.0</v>
+        <v>465.0</v>
       </c>
     </row>
     <row r="4">

</xml_diff>